<commit_message>
Update to A4 barcode sheet, 45x23mm
</commit_message>
<xml_diff>
--- a/sri_lanka/Sample Data.xlsx
+++ b/sri_lanka/Sample Data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Item category</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>Boots</t>
+  </si>
+  <si>
+    <t>Adidas wristband</t>
+  </si>
+  <si>
+    <t>Altus Yoga Mat</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Misc Clothing</t>
+  </si>
+  <si>
+    <t>Nike headband</t>
   </si>
 </sst>
 </file>
@@ -391,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -448,7 +463,7 @@
         <v>4500.8999999999996</v>
       </c>
       <c r="E3" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -465,7 +480,58 @@
         <v>2500.9</v>
       </c>
       <c r="E4" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1420</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1850.75</v>
+      </c>
+      <c r="E5" s="2">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2840</v>
+      </c>
+      <c r="D6" s="2">
+        <v>2200</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>9810304</v>
+      </c>
+      <c r="D7" s="2">
+        <v>8499.4</v>
+      </c>
+      <c r="E7" s="2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>